<commit_message>
reorganise info on projects page
</commit_message>
<xml_diff>
--- a/_data/publications.xlsx
+++ b/_data/publications.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ulyngs/Library/Mobile Documents/com~apple~CloudDocs/Website/lyngs-hugo/_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE4429B-F1C7-3A47-99EB-3A37606588B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35958B25-0E75-3D4B-89B5-24DFB03BDEDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{658FACE9-883F-4F49-B936-65547CAA7E51}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="125">
   <si>
     <t>type</t>
   </si>
@@ -78,15 +78,9 @@
     <t>url</t>
   </si>
   <si>
-    <t>https://ulriklyngs.com/publications</t>
-  </si>
-  <si>
     <t>https://dl.acm.org/citation.cfm?doid=3201064.3201089</t>
   </si>
   <si>
-    <t>https://dl.acm.org/citation.cfm?id=3188397</t>
-  </si>
-  <si>
     <t>https://dl.acm.org/citation.cfm?id=3173951</t>
   </si>
   <si>
@@ -207,42 +201,6 @@
     <t>pdf</t>
   </si>
   <si>
-    <t>Lyngs2019_preprint_2019_mar_03.pdf</t>
-  </si>
-  <si>
-    <t>Lyngs2019_workshop_digi_wellbeing_submission_camera_ready</t>
-  </si>
-  <si>
-    <t>Lyngs2016_rel_self_control_MA_thesis</t>
-  </si>
-  <si>
-    <t>Zhao_et_al_2018_KOALA_report_m3</t>
-  </si>
-  <si>
-    <t>Lyngs2018_cog_ design_space</t>
-  </si>
-  <si>
-    <t>Lyngs2018_what_users_want</t>
-  </si>
-  <si>
-    <t>Lyngs2016_hearing_in_color</t>
-  </si>
-  <si>
-    <t>Lyngs2019_curiosity</t>
-  </si>
-  <si>
-    <t>Binns_et_al_2018_3rd_party_tracking_in_mobile_eco</t>
-  </si>
-  <si>
-    <t>Binns_et_al_2018_ algo_justice</t>
-  </si>
-  <si>
-    <t>Lyngs2017_smartphone_distraction_chi</t>
-  </si>
-  <si>
-    <t>Lyngs_McKay2017_smartphone_distraction_cogsci</t>
-  </si>
-  <si>
     <t>materials</t>
   </si>
   <si>
@@ -270,9 +228,6 @@
     <t>desat_matrix.jpg</t>
   </si>
   <si>
-    <t>https://ulriklyngs.com/file/102/download?token=YRZoq5qR</t>
-  </si>
-  <si>
     <t>CHI’19 Workshop: Designing for Digital Wellbeing</t>
   </si>
   <si>
@@ -391,6 +346,66 @@
   </si>
   <si>
     <t>redd-workshop</t>
+  </si>
+  <si>
+    <t>/pdfs/2020-02-20_Lyngs_CHI2020_workshop_rethinking_mental_health.pdf</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/pdf/2001.04180.pdf</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/pdf/1902.00157.pdf</t>
+  </si>
+  <si>
+    <t>CHI'19 workshop</t>
+  </si>
+  <si>
+    <t>/pdfs/2019-02-08_Lyngs_workshop_digi_wellbeing.pdf</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/pdf/1803.02065.pdf</t>
+  </si>
+  <si>
+    <t>https://dl.acm.org/doi/10.1145/3170427.3188397</t>
+  </si>
+  <si>
+    <t>https://dl.acm.org/doi/10.1145/3290605.3300361</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/pdf/1804.03603.pdf</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/pdf/1801.10408.pdf</t>
+  </si>
+  <si>
+    <t>/pdfs/2018-04_Lyngs_cog_design_space.pdf</t>
+  </si>
+  <si>
+    <t>/pdfs/2017_lyngs_mckay_cell_perf_cogsci.pdf</t>
+  </si>
+  <si>
+    <t>/pdfs/2016_lyngs_hearing_color.pdf</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/pdf/1809.10841.pdf</t>
+  </si>
+  <si>
+    <t>/pdfs/2017_lyngs_curiousity_attention_chi_workshop.pdf</t>
+  </si>
+  <si>
+    <t>/pdfs/2016_lyngs_ma_thesis_cultural_self_control.pdf</t>
+  </si>
+  <si>
+    <t>/pdfs/2017_lyngs_cell_perf_chi_ea.pdf</t>
+  </si>
+  <si>
+    <t>JEP:HPP</t>
+  </si>
+  <si>
+    <t>Report</t>
+  </si>
+  <si>
+    <t>MA Thesis</t>
   </si>
 </sst>
 </file>
@@ -762,10 +777,10 @@
   <dimension ref="A1:S17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -784,7 +799,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -793,176 +808,179 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J1" t="s">
         <v>14</v>
       </c>
       <c r="K1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M1" t="s">
         <v>57</v>
       </c>
-      <c r="L1" t="s">
-        <v>70</v>
-      </c>
-      <c r="M1" t="s">
-        <v>71</v>
-      </c>
       <c r="N1" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="O1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="P1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Q1" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="R1" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="S1" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="C2">
         <v>2020</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="E2" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="G2" t="s">
-        <v>118</v>
+        <v>103</v>
+      </c>
+      <c r="K2" t="s">
+        <v>105</v>
       </c>
       <c r="S2" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="68" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="C3">
         <v>2020</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="E3" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="G3" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="68" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="C4">
         <v>2020</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="G4" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="102" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="C5">
         <v>2020</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="E5" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="G5" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="H5" t="s">
-        <v>84</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K5" s="1"/>
+        <v>69</v>
+      </c>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="L5" s="1" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="P5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="Q5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="S5" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="85" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C6">
         <v>2019</v>
@@ -971,51 +989,51 @@
         <v>4</v>
       </c>
       <c r="E6" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="G6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>15</v>
+        <v>112</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>58</v>
+        <v>107</v>
       </c>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="P6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="Q6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="R6" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="S6" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C7">
         <v>2018</v>
@@ -1024,45 +1042,45 @@
         <v>5</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="G7" t="s">
         <v>6</v>
       </c>
       <c r="H7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I7" t="s">
         <v>7</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>66</v>
+        <v>113</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="P7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="Q7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="R7" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C8">
         <v>2018</v>
@@ -1071,39 +1089,39 @@
         <v>8</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="G8" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="H8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>63</v>
+        <v>110</v>
       </c>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="P8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="S8" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="68" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C9">
         <v>2018</v>
@@ -1112,74 +1130,74 @@
         <v>9</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="G9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>67</v>
+        <v>114</v>
       </c>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="P9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="68" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C10">
         <v>2018</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="G10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>62</v>
+        <v>115</v>
       </c>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="S10" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="85" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="C11">
         <v>2017</v>
@@ -1188,7 +1206,7 @@
         <v>10</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="G11" t="s">
         <v>11</v>
@@ -1197,30 +1215,30 @@
         <v>11</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>69</v>
+        <v>116</v>
       </c>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="P11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="S11" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="C12">
         <v>2016</v>
@@ -1228,6 +1246,9 @@
       <c r="D12" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="F12" s="2" t="s">
+        <v>122</v>
+      </c>
       <c r="G12" t="s">
         <v>13</v>
       </c>
@@ -1235,45 +1256,48 @@
         <v>13</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>64</v>
+        <v>117</v>
       </c>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="P12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="S12" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:19" ht="85" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C13">
         <v>2018</v>
       </c>
       <c r="D13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="G13" t="s">
+        <v>24</v>
+      </c>
+      <c r="J13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G13" t="s">
-        <v>26</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="K13" s="1" t="s">
-        <v>61</v>
+        <v>118</v>
       </c>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
@@ -1281,127 +1305,128 @@
     </row>
     <row r="14" spans="1:19" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C14">
         <v>2017</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="G14" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>65</v>
+        <v>119</v>
       </c>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="S14" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:19" ht="68" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C15">
         <v>2016</v>
       </c>
       <c r="D15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="G15" t="s">
+        <v>34</v>
+      </c>
+      <c r="J15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G15" t="s">
-        <v>36</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="K15" s="1" t="s">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
       <c r="S15" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:19" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C16">
         <v>2019</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="G16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H16" t="s">
-        <v>80</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>79</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="J16" s="1"/>
       <c r="K16" t="s">
-        <v>59</v>
+        <v>109</v>
       </c>
       <c r="O16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="P16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="S16" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="85" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C17">
         <v>2017</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="G17" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>68</v>
+        <v>121</v>
       </c>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
@@ -1411,18 +1436,22 @@
   <hyperlinks>
     <hyperlink ref="J6" r:id="rId1" xr:uid="{6EC5B298-2427-5747-A27C-098FCF271437}"/>
     <hyperlink ref="J7" r:id="rId2" xr:uid="{4259178C-1153-554C-A054-5CECA758F56D}"/>
-    <hyperlink ref="J8" r:id="rId3" xr:uid="{DA43A3E4-C374-CB47-97A0-E54F3FF1B69D}"/>
-    <hyperlink ref="J9" r:id="rId4" xr:uid="{4DCB5AF8-27E6-5C4F-BC66-7410E0A1DA33}"/>
-    <hyperlink ref="J10" r:id="rId5" xr:uid="{77F8AB0B-104B-1144-9115-997327C4BF00}"/>
-    <hyperlink ref="J11" r:id="rId6" xr:uid="{09D6C851-A176-8248-961E-FABBA12FAF46}"/>
-    <hyperlink ref="J12" r:id="rId7" xr:uid="{2DAB3535-1D8A-7543-9712-4C92AA4E1F8D}"/>
-    <hyperlink ref="J13" r:id="rId8" xr:uid="{E8DAA116-1175-AF47-9174-B814693897BB}"/>
-    <hyperlink ref="J14" r:id="rId9" xr:uid="{5081606E-AECD-0A4E-94AF-90AAD0F60FAD}"/>
-    <hyperlink ref="J15" r:id="rId10" xr:uid="{D80AF795-CEC7-2C48-ABD3-224438FFFD8C}"/>
-    <hyperlink ref="J17" r:id="rId11" xr:uid="{2C875ED6-7B5C-1040-8B19-F1CC72E718C1}"/>
-    <hyperlink ref="J16" r:id="rId12" xr:uid="{2BCD7964-E196-0441-9017-AF2FA366E6E2}"/>
-    <hyperlink ref="J5" r:id="rId13" xr:uid="{5A816734-7CFE-C34F-8731-58C85930E565}"/>
-    <hyperlink ref="L5" r:id="rId14" xr:uid="{0C9D072B-4E7E-2040-B4AF-6C0EDC74A174}"/>
+    <hyperlink ref="J9" r:id="rId3" xr:uid="{4DCB5AF8-27E6-5C4F-BC66-7410E0A1DA33}"/>
+    <hyperlink ref="J10" r:id="rId4" xr:uid="{77F8AB0B-104B-1144-9115-997327C4BF00}"/>
+    <hyperlink ref="J11" r:id="rId5" xr:uid="{09D6C851-A176-8248-961E-FABBA12FAF46}"/>
+    <hyperlink ref="J12" r:id="rId6" xr:uid="{2DAB3535-1D8A-7543-9712-4C92AA4E1F8D}"/>
+    <hyperlink ref="J13" r:id="rId7" xr:uid="{E8DAA116-1175-AF47-9174-B814693897BB}"/>
+    <hyperlink ref="J14" r:id="rId8" xr:uid="{5081606E-AECD-0A4E-94AF-90AAD0F60FAD}"/>
+    <hyperlink ref="J15" r:id="rId9" xr:uid="{D80AF795-CEC7-2C48-ABD3-224438FFFD8C}"/>
+    <hyperlink ref="J17" r:id="rId10" xr:uid="{2C875ED6-7B5C-1040-8B19-F1CC72E718C1}"/>
+    <hyperlink ref="L5" r:id="rId11" xr:uid="{0C9D072B-4E7E-2040-B4AF-6C0EDC74A174}"/>
+    <hyperlink ref="K8" r:id="rId12" xr:uid="{A7287BAE-5B52-3F4C-9C3E-23D534F0274D}"/>
+    <hyperlink ref="J8" r:id="rId13" xr:uid="{31D2AF80-F3A0-0541-A01A-56100A66E8B7}"/>
+    <hyperlink ref="K5" r:id="rId14" xr:uid="{69D7D62F-C493-2546-BE3D-3E82F6A9B8BC}"/>
+    <hyperlink ref="K6" r:id="rId15" xr:uid="{7EBE5EB6-D71C-BF47-BB62-50BC6DAB3E81}"/>
+    <hyperlink ref="K7" r:id="rId16" xr:uid="{3D81032B-520E-8241-B37D-7136299851D5}"/>
+    <hyperlink ref="K9" r:id="rId17" xr:uid="{01EB20AB-1BD5-D443-B43F-4B789032796A}"/>
+    <hyperlink ref="K13" r:id="rId18" xr:uid="{F9AB7822-8C0F-4649-9A49-6CFE428FAEBA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add content links to publications
</commit_message>
<xml_diff>
--- a/_data/publications.xlsx
+++ b/_data/publications.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ulyngs/Library/Mobile Documents/com~apple~CloudDocs/Website/lyngs-hugo/_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35958B25-0E75-3D4B-89B5-24DFB03BDEDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF0FECF-5291-D444-A9DA-5A23CAF6EBA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{658FACE9-883F-4F49-B936-65547CAA7E51}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="134">
   <si>
     <t>type</t>
   </si>
@@ -406,6 +406,33 @@
   </si>
   <si>
     <t>MA Thesis</t>
+  </si>
+  <si>
+    <t>blog</t>
+  </si>
+  <si>
+    <t>video</t>
+  </si>
+  <si>
+    <t>https://osf.io/ed3wh/</t>
+  </si>
+  <si>
+    <t>https://osf.io/4nu9e/</t>
+  </si>
+  <si>
+    <t>https://osf.io/5v8ua/</t>
+  </si>
+  <si>
+    <t>https://osf.io/hdvtm/</t>
+  </si>
+  <si>
+    <t>https://ulyngs.github.io/cog-design-space-ict-self-control/</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=sJf_F7faczU</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=m9YzuNI7uOc</t>
   </si>
 </sst>
 </file>
@@ -774,13 +801,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D849796-8D2F-2144-8637-FA01837A8DE5}">
-  <dimension ref="A1:S17"/>
+  <dimension ref="A1:U17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomRight" activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -794,7 +821,7 @@
     <col min="7" max="8" width="49.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -832,28 +859,34 @@
         <v>56</v>
       </c>
       <c r="M1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N1" t="s">
+        <v>125</v>
+      </c>
+      <c r="O1" t="s">
+        <v>126</v>
+      </c>
+      <c r="P1" t="s">
         <v>57</v>
       </c>
-      <c r="N1" t="s">
-        <v>58</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>21</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>42</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>59</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>62</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="85" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -878,11 +911,14 @@
       <c r="K2" t="s">
         <v>105</v>
       </c>
-      <c r="S2" t="s">
+      <c r="L2" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="U2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="68" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="68" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -908,7 +944,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="68" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" ht="68" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -928,7 +964,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="102" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" ht="102" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -962,20 +998,22 @@
       </c>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
-      <c r="O5" t="s">
-        <v>22</v>
-      </c>
-      <c r="P5" t="s">
-        <v>22</v>
-      </c>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
       <c r="Q5" t="s">
         <v>22</v>
       </c>
+      <c r="R5" t="s">
+        <v>22</v>
+      </c>
       <c r="S5" t="s">
+        <v>22</v>
+      </c>
+      <c r="U5" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="85" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" ht="85" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -1009,26 +1047,34 @@
       <c r="K6" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
+      <c r="L6" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>131</v>
+      </c>
       <c r="N6" s="1"/>
-      <c r="O6" t="s">
-        <v>22</v>
-      </c>
-      <c r="P6" t="s">
-        <v>22</v>
-      </c>
+      <c r="O6" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="P6" s="1"/>
       <c r="Q6" t="s">
         <v>22</v>
       </c>
       <c r="R6" t="s">
+        <v>22</v>
+      </c>
+      <c r="S6" t="s">
+        <v>22</v>
+      </c>
+      <c r="T6" t="s">
         <v>63</v>
       </c>
-      <c r="S6" t="s">
+      <c r="U6" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -1059,23 +1105,27 @@
       <c r="K7" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="L7" s="1"/>
+      <c r="L7" s="1" t="s">
+        <v>128</v>
+      </c>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
-      <c r="O7" t="s">
-        <v>22</v>
-      </c>
-      <c r="P7" t="s">
-        <v>22</v>
-      </c>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
       <c r="Q7" t="s">
         <v>22</v>
       </c>
       <c r="R7" t="s">
+        <v>22</v>
+      </c>
+      <c r="S7" t="s">
+        <v>22</v>
+      </c>
+      <c r="T7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -1103,20 +1153,24 @@
       <c r="K8" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="L8" s="1"/>
+      <c r="L8" s="1" t="s">
+        <v>129</v>
+      </c>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
-      <c r="O8" t="s">
-        <v>22</v>
-      </c>
-      <c r="P8" t="s">
-        <v>22</v>
-      </c>
-      <c r="S8" t="s">
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" t="s">
+        <v>22</v>
+      </c>
+      <c r="R8" t="s">
+        <v>22</v>
+      </c>
+      <c r="U8" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="68" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" ht="68" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -1147,14 +1201,18 @@
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
-      <c r="O9" t="s">
-        <v>22</v>
-      </c>
-      <c r="P9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" ht="68" x14ac:dyDescent="0.2">
+      <c r="O9" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="P9" s="1"/>
+      <c r="Q9" t="s">
+        <v>22</v>
+      </c>
+      <c r="R9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="68" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1185,14 +1243,16 @@
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
-      <c r="O10" t="s">
-        <v>22</v>
-      </c>
-      <c r="S10" t="s">
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" t="s">
+        <v>22</v>
+      </c>
+      <c r="U10" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="85" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" ht="85" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1223,17 +1283,19 @@
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
-      <c r="O11" t="s">
-        <v>22</v>
-      </c>
-      <c r="P11" t="s">
-        <v>22</v>
-      </c>
-      <c r="S11" t="s">
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" t="s">
+        <v>22</v>
+      </c>
+      <c r="R11" t="s">
+        <v>22</v>
+      </c>
+      <c r="U11" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -1264,17 +1326,19 @@
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
-      <c r="O12" t="s">
-        <v>22</v>
-      </c>
-      <c r="P12" t="s">
-        <v>22</v>
-      </c>
-      <c r="S12" t="s">
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" t="s">
+        <v>22</v>
+      </c>
+      <c r="R12" t="s">
+        <v>22</v>
+      </c>
+      <c r="U12" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="85" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" ht="85" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -1302,8 +1366,10 @@
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
-    </row>
-    <row r="14" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+    </row>
+    <row r="14" spans="1:21" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -1331,11 +1397,13 @@
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
-      <c r="S14" t="s">
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="U14" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="68" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" ht="68" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -1363,11 +1431,13 @@
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
-      <c r="S15" t="s">
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="U15" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -1393,17 +1463,17 @@
       <c r="K16" t="s">
         <v>109</v>
       </c>
-      <c r="O16" t="s">
-        <v>22</v>
-      </c>
-      <c r="P16" t="s">
-        <v>22</v>
-      </c>
-      <c r="S16" t="s">
+      <c r="Q16" t="s">
+        <v>22</v>
+      </c>
+      <c r="R16" t="s">
+        <v>22</v>
+      </c>
+      <c r="U16" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -1431,6 +1501,8 @@
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1452,6 +1524,13 @@
     <hyperlink ref="K7" r:id="rId16" xr:uid="{3D81032B-520E-8241-B37D-7136299851D5}"/>
     <hyperlink ref="K9" r:id="rId17" xr:uid="{01EB20AB-1BD5-D443-B43F-4B789032796A}"/>
     <hyperlink ref="K13" r:id="rId18" xr:uid="{F9AB7822-8C0F-4649-9A49-6CFE428FAEBA}"/>
+    <hyperlink ref="L6" r:id="rId19" xr:uid="{10E16F54-594C-444C-AA87-AE89D309077B}"/>
+    <hyperlink ref="L7" r:id="rId20" xr:uid="{8A6232DC-3480-D548-9BF8-8AF04803A917}"/>
+    <hyperlink ref="L8" r:id="rId21" xr:uid="{0C467AF9-4DA5-424E-AF93-D9BDC8D3BDC0}"/>
+    <hyperlink ref="L2" r:id="rId22" xr:uid="{47AA7309-BC6F-3E40-B69F-47F16A59DA45}"/>
+    <hyperlink ref="M6" r:id="rId23" xr:uid="{7A938748-1082-0945-ACAE-4CA66ABD1BDE}"/>
+    <hyperlink ref="O6" r:id="rId24" xr:uid="{B24E8AE9-AE1C-F94C-ACC3-BF5A7E62D73D}"/>
+    <hyperlink ref="O9" r:id="rId25" xr:uid="{14D6FD40-7DAE-2B42-A812-A4FC505C64D9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>